<commit_message>
adding new files to repository
</commit_message>
<xml_diff>
--- a/working/2034 planning.xlsx
+++ b/working/2034 planning.xlsx
@@ -1091,17 +1091,98 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100140A42B38915AC4EBAF791562DC92B4E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c471dd606aec017af3d5b7c6a4158e0a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b764bea3eb9b1a5be8fd57fac5fb459b">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100140A42B38915AC4EBAF791562DC92B4E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9782937a82cd0419a21f282f626a20cd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4" xmlns:ns3="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5341088267d3fc8603e8164504c16655" ns2:_="" ns3:_="">
+    <xsd:import namespace="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4"/>
+    <xsd:import namespace="0ffa7682-a752-4ec2-9b00-944c9a00bbe9"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
-              <xsd:all/>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="886477d7-ad29-47e7-b319-eaa6f1949674" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{4f3b23a9-39ee-43d8-8bbd-bfe89c769496}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="0ffa7682-a752-4ec2-9b00-944c9a00bbe9">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
@@ -1215,12 +1296,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41945E-BC49-470A-9D77-565233BB91B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AB33A3C-F309-4074-B4F4-58D42FD99226}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>